<commit_message>
Artefato 16 e 17
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos.xlsx
+++ b/17. Análise de Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\fabio\dev\impacta\3º Semestre\Engenharia de Requisito\Road.on\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriela\Documents\3  Semestre\OPE\RoadOn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F4FAE8-31C7-4F9F-925E-0489768A8BB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82534452-BB15-42AF-B060-4B45A4C82714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>Cliente solicita a adesão do plano de excursão</t>
   </si>
   <si>
-    <t xml:space="preserve">Cliente realiza pagamento da excursão ao financeiro </t>
-  </si>
-  <si>
     <t>Cliente NÃO realiza pagamento da excursão ao financeiro.</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>Gerente planeja excursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente realiza pagamento da excursão ao comercial </t>
   </si>
 </sst>
 </file>
@@ -367,6 +367,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -377,19 +386,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -815,15 +815,15 @@
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="4"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -833,20 +833,20 @@
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="4"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
@@ -875,10 +875,10 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6">
@@ -899,8 +899,8 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="6">
         <v>2</v>
       </c>
@@ -919,8 +919,8 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="6">
         <v>3</v>
       </c>
@@ -939,8 +939,8 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="6">
         <v>4</v>
       </c>
@@ -959,8 +959,8 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="6">
         <v>5</v>
       </c>
@@ -979,8 +979,8 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="6">
         <v>6</v>
       </c>
@@ -999,8 +999,8 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="23" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="6">
@@ -1021,8 +1021,8 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="6">
         <v>8</v>
       </c>
@@ -1041,10 +1041,10 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="6">
@@ -1065,8 +1065,8 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="26"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="6">
         <v>2</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="3:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1109,8 +1109,8 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="27"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="16">
@@ -1130,8 +1130,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="27"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="14">
         <v>3</v>
       </c>
@@ -1150,16 +1150,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1168,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:L25"/>
+  <dimension ref="B2:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,15 +1193,15 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="4"/>
       <c r="L2" s="1"/>
     </row>
@@ -1210,19 +1210,19 @@
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1250,17 +1250,17 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="18">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -1273,8 +1273,8 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="18">
         <v>2</v>
       </c>
@@ -1292,13 +1292,13 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="18">
         <v>3</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -1311,8 +1311,8 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="18">
         <v>4</v>
       </c>
@@ -1330,13 +1330,13 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="18">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>36</v>
@@ -1349,7 +1349,7 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="17" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1373,14 +1373,14 @@
       <c r="B11" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="18">
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>39</v>
@@ -1394,12 +1394,12 @@
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="30"/>
-      <c r="C12" s="29"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="19">
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>24</v>
@@ -1413,12 +1413,12 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
-      <c r="C13" s="29"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="19">
         <v>9</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1431,17 +1431,17 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="20">
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1454,13 +1454,13 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="29"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="20">
         <v>11</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>40</v>
@@ -1473,13 +1473,13 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="29"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="19">
         <v>12</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -1493,9 +1493,6 @@
     </row>
     <row r="21" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E21" s="21"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E25" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Artefato 17 atualizado após feedback
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos.xlsx
+++ b/17. Análise de Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\fabio\dev\impacta\3º Semestre\Engenharia de Requisito\Road.on\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbd7024f7b2b0faf/Documentos/GitCertoCarai/RoadOn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076BE73C-3B51-47A4-BCA0-C48DD7860A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{076BE73C-3B51-47A4-BCA0-C48DD7860A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FDF1417B-74A7-4C0D-BE41-E3B747E7B393}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="63">
   <si>
     <t>Externo</t>
   </si>
@@ -188,13 +188,40 @@
   </si>
   <si>
     <t>Cliente NÃO realiza pagamento da excursão ao comercial.</t>
+  </si>
+  <si>
+    <t>Informar detalhes pré excursão</t>
+  </si>
+  <si>
+    <t>Receber solicitação do cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cliente informa a solicitação de cancelamento da excursão</t>
+  </si>
+  <si>
+    <t>Informar detalhes durante a excursão</t>
+  </si>
+  <si>
+    <t>x(12)</t>
+  </si>
+  <si>
+    <t>Gerente apresenta as informações da pré-excursão para o cliente</t>
+  </si>
+  <si>
+    <t>Gerente envia o cancelamento da excursão</t>
+  </si>
+  <si>
+    <t>Gerente disponibiliza o plano de excursão ao cliente durante a viagem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -228,8 +255,17 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +320,32 @@
         <bgColor rgb="FFB4C7E7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF0066CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE8F62"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -308,11 +368,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -354,19 +427,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -377,22 +459,37 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,6 +564,12 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFE8F62"/>
+      <color rgb="FFA60638"/>
+      <color rgb="FFD69AB1"/>
+      <color rgb="FF410B23"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -815,15 +918,15 @@
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
       <c r="L3" s="4"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -833,20 +936,20 @@
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="4"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
@@ -875,10 +978,10 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6">
@@ -899,8 +1002,8 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="6">
         <v>2</v>
       </c>
@@ -919,8 +1022,8 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="6">
         <v>3</v>
       </c>
@@ -939,8 +1042,8 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="6">
         <v>4</v>
       </c>
@@ -959,8 +1062,8 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="6">
         <v>5</v>
       </c>
@@ -979,8 +1082,8 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="6">
         <v>6</v>
       </c>
@@ -999,8 +1102,8 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="24"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="23" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="6">
@@ -1021,8 +1124,8 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="6">
         <v>8</v>
       </c>
@@ -1041,10 +1144,10 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="6">
@@ -1065,8 +1168,8 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="26"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="6">
         <v>2</v>
       </c>
@@ -1085,7 +1188,7 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="3:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1109,8 +1212,8 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="27"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="16">
@@ -1130,8 +1233,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="27"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="14">
         <v>3</v>
       </c>
@@ -1150,16 +1253,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:K4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:C13"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="G3:H4"/>
-    <mergeCell ref="I3:K4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:C13"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1168,17 +1271,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:L21"/>
+  <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="38" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="86" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -1191,38 +1294,38 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22" t="s">
+      <c r="G2" s="25"/>
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="4"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1256,7 +1359,7 @@
       <c r="C5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -1275,7 +1378,7 @@
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="29"/>
       <c r="C6" s="28"/>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1294,7 +1397,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="29"/>
       <c r="C7" s="28"/>
-      <c r="D7" s="18">
+      <c r="D7" s="17">
         <v>3</v>
       </c>
       <c r="E7" s="12" t="s">
@@ -1313,7 +1416,7 @@
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="29"/>
       <c r="C8" s="28"/>
-      <c r="D8" s="18">
+      <c r="D8" s="17">
         <v>4</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1332,7 +1435,7 @@
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="29"/>
       <c r="C9" s="28"/>
-      <c r="D9" s="18">
+      <c r="D9" s="17">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -1350,10 +1453,10 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="29"/>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>6</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -1370,13 +1473,13 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="17">
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
@@ -1393,9 +1496,9 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="28"/>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -1412,9 +1515,9 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="28"/>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>9</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -1430,18 +1533,18 @@
       <c r="K13" s="10"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="28" t="s">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="18">
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1451,53 +1554,145 @@
       <c r="K14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="20">
+      <c r="L14" s="11"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="18">
         <v>11</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="L15" s="11"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="19">
+    <row r="16" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="30"/>
+      <c r="C16" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="18">
         <v>12</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>49</v>
+      <c r="E16" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="21"/>
+      <c r="L16" s="11"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="18">
+        <v>13</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="19">
+        <v>14</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="19">
+        <v>15</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="18">
+        <v>16</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E25" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
+  <mergeCells count="10">
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
     <mergeCell ref="F2:G3"/>
     <mergeCell ref="H2:J3"/>
     <mergeCell ref="B4:C4"/>
@@ -1505,6 +1700,7 @@
     <mergeCell ref="C5:C9"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B15:B16"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Manutenção artefato 17 e 18
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos.xlsx
+++ b/17. Análise de Eventos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbd7024f7b2b0faf/Documentos/GitCertoCarai/RoadOn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\fabio\dev\impacta\3º Semestre\Engenharia de Requisito\Road.on\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{076BE73C-3B51-47A4-BCA0-C48DD7860A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FDF1417B-74A7-4C0D-BE41-E3B747E7B393}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D00C9C-CA4B-4E85-B995-C63FA8997A8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="2130" windowWidth="21600" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>x(4,5)</t>
   </si>
   <si>
-    <t>x(10)</t>
-  </si>
-  <si>
     <t>x(11)</t>
   </si>
   <si>
@@ -199,22 +196,25 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Cliente informa a solicitação de cancelamento da excursão</t>
-  </si>
-  <si>
     <t>Informar detalhes durante a excursão</t>
   </si>
   <si>
-    <t>x(12)</t>
-  </si>
-  <si>
-    <t>Gerente apresenta as informações da pré-excursão para o cliente</t>
-  </si>
-  <si>
-    <t>Gerente envia o cancelamento da excursão</t>
-  </si>
-  <si>
-    <t>Gerente disponibiliza o plano de excursão ao cliente durante a viagem</t>
+    <t>x(14)</t>
+  </si>
+  <si>
+    <t>x(15)</t>
+  </si>
+  <si>
+    <t>Atendente disponibiliza o plano de excursão para o cliente antes da viagem</t>
+  </si>
+  <si>
+    <t>Cliente realiza solicitação de acordo com imprevisto</t>
+  </si>
+  <si>
+    <t>Atendente comunica cancelamento da excursão ao Gerente</t>
+  </si>
+  <si>
+    <t>Atendente disponibiliza informações durante excursão</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -440,22 +440,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -464,32 +488,11 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,15 +921,15 @@
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="29"/>
+      <c r="I3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="4"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -936,20 +939,20 @@
       <c r="D4" s="2"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="4"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="26"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
@@ -978,10 +981,10 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6">
@@ -1002,8 +1005,8 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="27"/>
-      <c r="D7" s="23"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="6">
         <v>2</v>
       </c>
@@ -1022,8 +1025,8 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="27"/>
-      <c r="D8" s="23"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="6">
         <v>3</v>
       </c>
@@ -1042,8 +1045,8 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="27"/>
-      <c r="D9" s="23"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="6">
         <v>4</v>
       </c>
@@ -1062,8 +1065,8 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="27"/>
-      <c r="D10" s="23"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="6">
         <v>5</v>
       </c>
@@ -1082,8 +1085,8 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="27"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="6">
         <v>6</v>
       </c>
@@ -1102,8 +1105,8 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="27"/>
-      <c r="D12" s="23" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="32" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="6">
@@ -1124,8 +1127,8 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
-      <c r="D13" s="23"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="6">
         <v>8</v>
       </c>
@@ -1144,10 +1147,10 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="3:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="6">
@@ -1168,8 +1171,8 @@
       <c r="N14" s="1"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="6">
         <v>2</v>
       </c>
@@ -1188,7 +1191,7 @@
       <c r="N15" s="1"/>
     </row>
     <row r="16" spans="3:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="34" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="13" t="s">
@@ -1212,8 +1215,8 @@
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="24"/>
-      <c r="D17" s="23" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="16">
@@ -1233,8 +1236,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C18" s="24"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="14">
         <v>3</v>
       </c>
@@ -1253,16 +1256,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="G3:H4"/>
     <mergeCell ref="I3:K4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:C13"/>
     <mergeCell ref="D6:D11"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="G3:H4"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1273,15 +1276,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="28" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="86" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -1294,38 +1297,38 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
-      <c r="C2" s="37"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="1"/>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="4"/>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="37"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="1"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1353,17 +1356,17 @@
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="36" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="17">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -1376,13 +1379,13 @@
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="29"/>
-      <c r="C6" s="28"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="17">
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>18</v>
@@ -1395,13 +1398,13 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
-      <c r="C7" s="28"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="17">
         <v>3</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
@@ -1414,13 +1417,13 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="28"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="17">
         <v>4</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>38</v>
@@ -1433,13 +1436,13 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
-      <c r="C9" s="28"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="17">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>36</v>
@@ -1452,7 +1455,7 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="21" t="s">
         <v>25</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -1473,17 +1476,17 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="36" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="17">
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>39</v>
@@ -1496,13 +1499,13 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="18">
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>24</v>
@@ -1515,13 +1518,13 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="18">
         <v>9</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1534,17 +1537,17 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="18">
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
@@ -1557,20 +1560,20 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="18">
         <v>11</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="9"/>
@@ -1582,7 +1585,7 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="21" t="s">
         <v>25</v>
       </c>
@@ -1595,7 +1598,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -1603,16 +1606,16 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="32" t="s">
+      <c r="B17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="24" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="18">
         <v>13</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="25" t="s">
         <v>62</v>
       </c>
       <c r="F17" s="8" t="s">
@@ -1626,17 +1629,17 @@
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="36" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="19">
         <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1649,16 +1652,16 @@
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
-      <c r="C19" s="28"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="19">
         <v>15</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="9"/>
@@ -1668,18 +1671,18 @@
       <c r="L19" s="11"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="28"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="18">
         <v>16</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="9" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>

</xml_diff>

<commit_message>
Correção dos artefatos 3, 7, 9, 12, 13, 14, 17 e 21
</commit_message>
<xml_diff>
--- a/17. Análise de Eventos.xlsx
+++ b/17. Análise de Eventos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
   <si>
     <t xml:space="preserve">Externo</t>
   </si>
@@ -131,37 +131,37 @@
     <t xml:space="preserve">Cliente recebe agradecimentos  caso o feedback seja positivo.</t>
   </si>
   <si>
+    <t xml:space="preserve">Gerente planeja excursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parceiro envia informações solicitadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agente de vendas disponibiliza excursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente solicita a adesão do plano de excursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente realiza pagamento da excursão ao comercial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente NÃO realiza pagamento da excursão ao comercial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informar detalhes pré excursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atendente disponibiliza o plano de excursão para o cliente antes da viagem</t>
+  </si>
+  <si>
     <t xml:space="preserve">Receber solicitação do cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerente planeja excursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parceiro envia informações solicitadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agente de vendas disponibiliza excursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cliente solicita a adesão do plano de excursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cliente realiza pagamento da excursão ao comercial </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x(4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cliente NÃO realiza pagamento da excursão ao comercial.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informar detalhes pré excursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atendente disponibiliza o plano de excursão para o cliente antes da viagem</t>
   </si>
   <si>
     <t xml:space="preserve">Cliente solicita o cancelamento da excursão.</t>
@@ -615,7 +615,7 @@
       <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="2.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.57"/>
@@ -1012,10 +1012,10 @@
   <dimension ref="B1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54"/>
@@ -1031,9 +1031,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="21" t="s">
-        <v>36</v>
-      </c>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="2"/>
@@ -1106,7 +1104,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -1125,7 +1123,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>18</v>
@@ -1144,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1163,10 +1161,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="13"/>
@@ -1182,10 +1180,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>43</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="13"/>
@@ -1203,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1217,7 +1215,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>12</v>
@@ -1226,7 +1224,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1240,7 +1238,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="28" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>25</v>

</xml_diff>